<commit_message>
TopRecette : Doc + changement nom de bases
</commit_message>
<xml_diff>
--- a/docs/PlanDeTest.xlsx
+++ b/docs/PlanDeTest.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
   <si>
     <t>Plan de test</t>
   </si>
@@ -57,32 +57,71 @@
     <t>T0007</t>
   </si>
   <si>
-    <t>Modification d'un(e) jeu/console</t>
-  </si>
-  <si>
-    <t>Affichage d'une console /d'un jeu</t>
-  </si>
-  <si>
-    <t>Affichage de la liste des consoles / jeux</t>
-  </si>
-  <si>
-    <t>Recherche d'une console/ d'une jeu</t>
-  </si>
-  <si>
-    <t>Supprimer une console/ un jeu</t>
-  </si>
-  <si>
     <t>Rechercher une recette</t>
   </si>
   <si>
-    <t>Trier les recette</t>
+    <t>Modifier un recette</t>
+  </si>
+  <si>
+    <t>Supprimer une recette</t>
+  </si>
+  <si>
+    <t>Commenter et noter une recette</t>
+  </si>
+  <si>
+    <t>T0008</t>
+  </si>
+  <si>
+    <t>Trier les recettes</t>
+  </si>
+  <si>
+    <t>T0009</t>
+  </si>
+  <si>
+    <t>Créer un utilisateur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ajouter une recette sans / avec image </t>
+  </si>
+  <si>
+    <t>La recette est supprimée, les associations avec les ingéredients et leurs quantités sont supprimés, les comentaires / notes sont supprimés</t>
+  </si>
+  <si>
+    <t>Consulter un recette</t>
+  </si>
+  <si>
+    <t>Afficher la liste des recettes</t>
+  </si>
+  <si>
+    <t>T0010</t>
+  </si>
+  <si>
+    <t>T0011</t>
+  </si>
+  <si>
+    <t>T0012</t>
+  </si>
+  <si>
+    <t>T0013</t>
+  </si>
+  <si>
+    <t>T0014</t>
+  </si>
+  <si>
+    <t>T0015</t>
+  </si>
+  <si>
+    <t>L'image, les ingrédients et leur quantités, la préparation, l'orgine,</t>
+  </si>
+  <si>
+    <t>Supprimer son commentaire</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,6 +149,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -125,7 +172,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -224,16 +271,14 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
+      <left style="thin">
         <color auto="1"/>
       </left>
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thick">
+      <top/>
+      <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -242,28 +287,11 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="thin">
+      <right style="thick">
         <color auto="1"/>
       </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thick">
+      <top/>
+      <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -272,7 +300,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -300,21 +328,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -322,28 +335,37 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -649,24 +671,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E21"/>
+  <dimension ref="B2:E29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="15.85546875" customWidth="1"/>
-    <col min="4" max="4" width="64.28515625" customWidth="1"/>
-    <col min="5" max="5" width="60.85546875" customWidth="1"/>
+    <col min="4" max="4" width="36.85546875" customWidth="1"/>
+    <col min="5" max="5" width="66.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="C2" s="25" t="s">
+      <c r="B2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="25"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
     </row>
     <row r="3" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4"/>
@@ -675,164 +699,254 @@
       <c r="E3" s="4"/>
     </row>
     <row r="4" spans="2:5" ht="21.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="23" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="11"/>
+      <c r="D5" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="6" spans="2:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="19"/>
-    </row>
-    <row r="7" spans="2:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="20"/>
+    </row>
+    <row r="7" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="11"/>
-    </row>
-    <row r="8" spans="2:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="16" t="s">
+      <c r="E7" s="16"/>
+    </row>
+    <row r="8" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="19"/>
-    </row>
-    <row r="9" spans="2:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="17"/>
+    </row>
+    <row r="9" spans="2:5" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="16"/>
+    </row>
+    <row r="10" spans="2:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="17"/>
+    </row>
+    <row r="11" spans="2:5" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="12"/>
-    </row>
-    <row r="10" spans="2:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="18" t="s">
+      <c r="E11" s="18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="19"/>
-    </row>
-    <row r="11" spans="2:5" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="24"/>
-    </row>
-    <row r="12" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-    </row>
-    <row r="13" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="5"/>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="5"/>
-    </row>
-    <row r="15" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="5"/>
-    </row>
-    <row r="16" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="5"/>
-    </row>
-    <row r="17" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="5"/>
-    </row>
-    <row r="18" spans="2:5" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="2:5" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="2:5" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="2:5" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="1"/>
+      <c r="E12" s="17"/>
+    </row>
+    <row r="13" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="16"/>
+    </row>
+    <row r="14" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="17"/>
+    </row>
+    <row r="15" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="E15" s="16"/>
+    </row>
+    <row r="16" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="13"/>
+      <c r="E16" s="17"/>
+    </row>
+    <row r="17" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="9"/>
+      <c r="E17" s="16"/>
+    </row>
+    <row r="18" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="13"/>
+      <c r="E18" s="17"/>
+    </row>
+    <row r="19" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="9"/>
+      <c r="E19" s="16"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+    </row>
+    <row r="21" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="5"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="5"/>
+    </row>
+    <row r="23" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="5"/>
+    </row>
+    <row r="24" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="5"/>
+    </row>
+    <row r="25" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="5"/>
+    </row>
+    <row r="26" spans="2:5" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="2:5" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="2:5" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="2:5" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="B2:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
TopRecettes : doc technique + mcd
</commit_message>
<xml_diff>
--- a/docs/PlanDeTest.xlsx
+++ b/docs/PlanDeTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="-120" windowWidth="19635" windowHeight="12435"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="19635" windowHeight="10380"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="48">
   <si>
     <t>Plan de test</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Rechercher une recette</t>
   </si>
   <si>
-    <t>Modifier un recette</t>
-  </si>
-  <si>
     <t>Supprimer une recette</t>
   </si>
   <si>
@@ -78,15 +75,6 @@
     <t>T0009</t>
   </si>
   <si>
-    <t>Créer un utilisateur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ajouter une recette sans / avec image </t>
-  </si>
-  <si>
-    <t>La recette est supprimée, les associations avec les ingéredients et leurs quantités sont supprimés, les comentaires / notes sont supprimés</t>
-  </si>
-  <si>
     <t>Consulter un recette</t>
   </si>
   <si>
@@ -108,13 +96,70 @@
     <t>T0014</t>
   </si>
   <si>
-    <t>T0015</t>
-  </si>
-  <si>
-    <t>L'image, les ingrédients et leur quantités, la préparation, l'orgine,</t>
-  </si>
-  <si>
     <t>Supprimer son commentaire</t>
+  </si>
+  <si>
+    <t>Les recettes sont affichées selon le tri sélectionné</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ajouter une recette sans image </t>
+  </si>
+  <si>
+    <t xml:space="preserve">La recette est ajoutée correctement avec l'image par défaut </t>
+  </si>
+  <si>
+    <t>Modifier un recette avec une nouvelle image</t>
+  </si>
+  <si>
+    <t>L'ancienne image est supprimée seulement si elle avait étée ajoutée par l'utilisateur, la nouvelle image est uploadée et la recette est modifiée</t>
+  </si>
+  <si>
+    <t>Créer un utilisateur avec un peudo déjà utilisé</t>
+  </si>
+  <si>
+    <t>Le commentaire et la note associée au commentaire sont supprimés</t>
+  </si>
+  <si>
+    <t>Un message d'erreur apparaît pour en informer l'utilisateur, le compte n'est pas créé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le commentaire et la note sont ajoutés </t>
+  </si>
+  <si>
+    <t>L'image, les ingrédients et leur quantitée, la préparation, l'orgine, l'auteur, la note et les commentaire sont affiché</t>
+  </si>
+  <si>
+    <t>Accès à une recette qui n'existe pas</t>
+  </si>
+  <si>
+    <t>L'utilisateur est redirigé à la page de la liste des recettes</t>
+  </si>
+  <si>
+    <t>Un message d'erreur, La page de modification est rechergée en page d'ajout de recette</t>
+  </si>
+  <si>
+    <t>Toutes les recettes sont affichées</t>
+  </si>
+  <si>
+    <t>Supprimer un utilisateur</t>
+  </si>
+  <si>
+    <t>L'utilisateur est supprimé, les liens avec ses recettes sont supprimés et les commentaires/note qu'il a posté sont supprimés</t>
+  </si>
+  <si>
+    <t>Les recettes affichées ont une correspondance dans le titre avec la recherche</t>
+  </si>
+  <si>
+    <t>La recette est supprimée, le contenu (ingrédients, quantités)est supprimé, les comentaires / notes sont supprimés</t>
+  </si>
+  <si>
+    <t>Choisir un ingrédient qui n'est pas dans la base lors de l'ajout / modification d'une recette</t>
+  </si>
+  <si>
+    <t>L'ingrédient est ajouté dans la base</t>
+  </si>
+  <si>
+    <t>Modifier un recette sans en être le propriétaire</t>
   </si>
 </sst>
 </file>
@@ -172,7 +217,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -181,13 +226,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
+      <left style="thin">
         <color auto="1"/>
       </left>
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="thick">
+      <top style="thin">
         <color auto="1"/>
       </top>
       <bottom style="thin">
@@ -202,8 +247,21 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="thick">
-        <color auto="1"/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
         <color auto="1"/>
@@ -214,11 +272,11 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top style="thick">
-        <color auto="1"/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
         <color auto="1"/>
@@ -226,14 +284,14 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
         <color auto="1"/>
@@ -241,8 +299,8 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
+      <left style="medium">
+        <color indexed="64"/>
       </left>
       <right style="thin">
         <color auto="1"/>
@@ -259,8 +317,8 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="thick">
-        <color auto="1"/>
+      <right style="medium">
+        <color indexed="64"/>
       </right>
       <top style="thin">
         <color auto="1"/>
@@ -274,8 +332,8 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="thin">
-        <color auto="1"/>
+      <right style="medium">
+        <color indexed="64"/>
       </right>
       <top/>
       <bottom style="thin">
@@ -284,23 +342,94 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -319,53 +448,71 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -671,26 +818,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E29"/>
+  <dimension ref="B2:E27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="15.85546875" customWidth="1"/>
-    <col min="4" max="4" width="36.85546875" customWidth="1"/>
-    <col min="5" max="5" width="66.5703125" customWidth="1"/>
+    <col min="4" max="4" width="48.140625" customWidth="1"/>
+    <col min="5" max="5" width="79.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
     </row>
     <row r="3" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4"/>
@@ -698,197 +845,227 @@
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="2:5" ht="21.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="21" t="s">
+    <row r="4" spans="2:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="15" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="8" t="s">
+    <row r="5" spans="2:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="9" t="s">
+      <c r="C5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="16" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="19" t="s">
+      <c r="C16" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="20"/>
-    </row>
-    <row r="7" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="16"/>
-    </row>
-    <row r="8" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="17"/>
-    </row>
-    <row r="9" spans="2:5" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="16"/>
-    </row>
-    <row r="10" spans="2:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="17"/>
-    </row>
-    <row r="11" spans="2:5" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="17"/>
-    </row>
-    <row r="13" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" s="16"/>
-    </row>
-    <row r="14" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="11" t="s">
+      <c r="C17" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17" s="24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" s="17"/>
-    </row>
-    <row r="15" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="16"/>
-    </row>
-    <row r="16" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="17"/>
-    </row>
-    <row r="17" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="9"/>
-      <c r="E17" s="16"/>
-    </row>
-    <row r="18" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="13"/>
-      <c r="E18" s="17"/>
-    </row>
-    <row r="19" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="16"/>
+      <c r="C18" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18" s="27" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="5"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="5"/>
     </row>
     <row r="21" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B21" s="5"/>
@@ -896,10 +1073,10 @@
       <c r="D21" s="6"/>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
-      <c r="D22" s="7"/>
+      <c r="D22" s="6"/>
       <c r="E22" s="5"/>
     </row>
     <row r="23" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -908,17 +1085,17 @@
       <c r="D23" s="6"/>
       <c r="E23" s="5"/>
     </row>
-    <row r="24" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="5"/>
-    </row>
-    <row r="25" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="5"/>
+    <row r="24" spans="2:5" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="2:5" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="1"/>
     </row>
     <row r="26" spans="2:5" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
@@ -931,18 +1108,6 @@
       <c r="C27" s="1"/>
       <c r="D27" s="2"/>
       <c r="E27" s="1"/>
-    </row>
-    <row r="28" spans="2:5" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="1"/>
-    </row>
-    <row r="29" spans="2:5" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>